<commit_message>
Update N1, N2, P2, P2
</commit_message>
<xml_diff>
--- a/Test Data/SauceDemoApp_Nama Kalian.xlsx
+++ b/Test Data/SauceDemoApp_Nama Kalian.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fachry Ramadhan\git\SauceDemoAppTogetherLearn\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diska\git\SauceDemoAppTogetherLearn\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2BE635-D320-4C84-8F75-236033C60A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530C38A0-A466-49C7-B9A3-DA2D3C676AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>ItemName</t>
-  </si>
-  <si>
-    <t>standard_user</t>
   </si>
   <si>
     <t>secret_sauce</t>
@@ -486,7 +483,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +540,7 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -597,12 +594,8 @@
       <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>

</xml_diff>